<commit_message>
Expansion factors for ASCs
</commit_message>
<xml_diff>
--- a/R_Logit_Models/Location_Choice/Expanded/Exp_Comparison.xlsx
+++ b/R_Logit_Models/Location_Choice/Expanded/Exp_Comparison.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\R_Logit_Models\Location_Choice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\R_Logit_Models\Location_Choice\Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{297594EA-635A-4E69-A211-16326F7C6A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFFEE04-BE02-474C-A379-6C090B446E5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp_Comparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="13">
   <si>
     <t>Ref.</t>
   </si>
@@ -64,11 +72,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -545,12 +559,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -905,58 +921,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:F23"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2">
         <v>2</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2">
         <v>3</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2">
         <v>4</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2">
         <v>5</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1">
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2">
         <v>6</v>
       </c>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -1046,7 +1062,7 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>-0.25698446848024398</v>
@@ -1135,7 +1151,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>-1.8008494833828199</v>
@@ -1224,7 +1240,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2.6280720360159999</v>
@@ -1313,7 +1329,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-0.290568982879298</v>
@@ -1402,7 +1418,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>1.78575001591913</v>
@@ -1491,7 +1507,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1.26741450094605</v>
@@ -1846,137 +1862,1138 @@
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>0</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
+        <v>-0.25698446848024398</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-0.38664499971288602</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.35426314370053702</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.35426314370053702</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-1.8008494833828199</v>
+      </c>
+      <c r="I15" s="4">
+        <v>-2.2253222208994798</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-1.7711484542015301</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-1.7711484542015301</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2.6280720360159999</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2.9647290451049599</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2.9022209102374599</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>2.9022209102374599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1.1438956375812399</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.33025555702118</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.75473036244984</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.7998275389356599</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.18176099095613099</v>
+      </c>
+      <c r="I16" s="4">
+        <v>-6.5784924773903394E-2</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.207930227438761</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.29501297312884001</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2.3081366453846002</v>
+      </c>
+      <c r="O16" s="4">
+        <v>2.3906152476465601</v>
+      </c>
+      <c r="P16" s="4">
+        <v>2.5792749044697199</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>3.1354233285899902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.58167083727403801</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.80488651937779299</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.2121047404076299</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.3019445296411101</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-0.23790909243879699</v>
+      </c>
+      <c r="I17" s="4">
+        <v>-0.45860362543425398</v>
+      </c>
+      <c r="J17" s="4">
+        <v>-0.21013529039333001</v>
+      </c>
+      <c r="K17" s="4">
+        <v>-0.23551192998943599</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3">
+        <v>2</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.0386737172087499</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1.03831721498711</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1.3108815272169501</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1.7665814080764399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.80747569494791704</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.53726252520929</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.42520510373275</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.4618169605328899</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.637585541164985</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.17522055015439</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.66808324607557601</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.74476050168007402</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3">
+        <v>3</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1.87555210847854</v>
+      </c>
+      <c r="O18" s="4">
+        <v>2.9026608875843798</v>
+      </c>
+      <c r="P18" s="4">
+        <v>2.1499050311841699</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>2.6977600250644702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1.32256788365433</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.71720620934921397</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.9397540596052001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.5233320836247799</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.98530052126800405</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.43992478472158E-2</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1.0137418534127001</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.350510523540561</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3">
+        <v>4</v>
+      </c>
+      <c r="N19" s="4">
+        <v>3.2678061310076898</v>
+      </c>
+      <c r="O19" s="4">
+        <v>2.9068347762292102</v>
+      </c>
+      <c r="P19" s="4">
+        <v>3.5408108486571299</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>3.4201649499616802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2.02477599440454</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.46272801200574</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.68346928354807</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2.2514602468390099</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.34618580234552299</v>
+      </c>
+      <c r="I20" s="4">
+        <v>-0.55620454727197599</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.37396539611441998</v>
+      </c>
+      <c r="K20" s="4">
+        <v>-0.28710881208117101</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3">
+        <v>5</v>
+      </c>
+      <c r="N20" s="4">
+        <v>2.0557025620860898</v>
+      </c>
+      <c r="O20" s="4">
+        <v>1.7386330221618</v>
+      </c>
+      <c r="P20" s="4">
+        <v>2.3273493495837099</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>2.2093819664805201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4">
+        <v>-0.99505902159225201</v>
+      </c>
+      <c r="C21" s="4">
+        <v>-0.78932037483284201</v>
+      </c>
+      <c r="D21" s="4">
+        <v>-0.380234579236367</v>
+      </c>
+      <c r="E21" s="4">
+        <v>-0.75412464051138395</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <v>6</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1.3353178041151099</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.62646751939846101</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1.35565204651076</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.70215260068559404</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <v>2.2608327557419501</v>
+      </c>
+      <c r="O21" s="4">
+        <v>2.4761038899391599</v>
+      </c>
+      <c r="P21" s="4">
+        <v>2.5262331701174801</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>2.4143009198106302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4">
+        <v>-0.290568982879298</v>
+      </c>
+      <c r="C24" s="4">
+        <v>-0.53917223018427796</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5.2811854967900099E-2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5.2811854967900099E-2</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1.78575001591913</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2.0066630457018602</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1.97538495428438</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1.97538495428438</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1.26741450094605</v>
+      </c>
+      <c r="O24" s="4">
+        <v>1.24921357429794</v>
+      </c>
+      <c r="P24" s="4">
+        <v>1.8282705804486801</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>1.8282705804486801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1.4553502963095399</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1.4394739720487399</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.82808108435377</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1.10113634152109</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2.2942778798066401</v>
+      </c>
+      <c r="I25" s="4">
+        <v>2.1949177700506302</v>
+      </c>
+      <c r="J25" s="4">
+        <v>2.4804461598090501</v>
+      </c>
+      <c r="K25" s="4">
+        <v>4.6613307352843298</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4">
+        <v>2.15840320471826</v>
+      </c>
+      <c r="O25" s="4">
+        <v>2.4108032189389199</v>
+      </c>
+      <c r="P25" s="4">
+        <v>2.7264852844459599</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>3.5784010543518399</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.95568915686770795</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.86086466043854803</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.3221045433902301</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.114354160549969</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>1.9412040020031101</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1.86116497495342</v>
+      </c>
+      <c r="J26" s="4">
+        <v>2.13187371124295</v>
+      </c>
+      <c r="K26" s="4">
+        <v>4.1762787688882304</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3">
+        <v>2</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1.9708881083826699</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2.1807407253653799</v>
+      </c>
+      <c r="P26" s="4">
+        <v>2.5293539030104402</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>3.4167611279688499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>3</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1.24427130633712</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.85061344310767</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.6105924746399101</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.88093490793438001</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>3</v>
+      </c>
+      <c r="H27" s="4">
+        <v>2.7166342992356101</v>
+      </c>
+      <c r="I27" s="4">
+        <v>2.9221033220739798</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2.9072693995479599</v>
+      </c>
+      <c r="K27" s="4">
+        <v>5.0712884212206797</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="4">
+        <v>2.2778190243876102</v>
+      </c>
+      <c r="O27" s="4">
+        <v>2.5374386395291801</v>
+      </c>
+      <c r="P27" s="4">
+        <v>2.8502458739471099</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>3.6958753103886299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>4</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1.40396808174417</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.55348342014663099</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.7733251692154599</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1.1232352159904599</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
+        <v>4</v>
+      </c>
+      <c r="H28" s="4">
+        <v>4.9672753709764699</v>
+      </c>
+      <c r="I28" s="4">
+        <v>4.2779405649966504</v>
+      </c>
+      <c r="J28" s="4">
+        <v>5.15550029709462</v>
+      </c>
+      <c r="K28" s="4">
+        <v>4.9446191449204404</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3">
+        <v>4</v>
+      </c>
+      <c r="N28" s="4">
+        <v>3.7085104529806898</v>
+      </c>
+      <c r="O28" s="4">
+        <v>3.6294997311307902</v>
+      </c>
+      <c r="P28" s="4">
+        <v>4.2769473419384996</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>3.6793683758597799</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>5</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2.02925102274498</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.2393116916957601</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2.41863081369624</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1.74811917573813</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3">
+        <v>5</v>
+      </c>
+      <c r="H29" s="4">
+        <v>4.33485089321593</v>
+      </c>
+      <c r="I29" s="4">
+        <v>3.7127361481342001</v>
+      </c>
+      <c r="J29" s="4">
+        <v>4.5221959223713704</v>
+      </c>
+      <c r="K29" s="4">
+        <v>4.3152835304655497</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3">
+        <v>5</v>
+      </c>
+      <c r="N29" s="4">
+        <v>3.7488970308229099</v>
+      </c>
+      <c r="O29" s="4">
+        <v>3.7648299448561899</v>
+      </c>
+      <c r="P29" s="4">
+        <v>4.3132316322425401</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>3.7188865405649798</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4">
+        <v>-0.82131404454738799</v>
+      </c>
+      <c r="C30" s="4">
+        <v>-0.72964435008916095</v>
+      </c>
+      <c r="D30" s="4">
+        <v>-0.42681041816201398</v>
+      </c>
+      <c r="E30" s="4">
+        <v>-1.0796567221880999</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>6</v>
+      </c>
+      <c r="H30" s="4">
+        <v>4.07646701357372</v>
+      </c>
+      <c r="I30" s="4">
+        <v>3.4694364818655701</v>
+      </c>
+      <c r="J30" s="4">
+        <v>4.2569183041039604</v>
+      </c>
+      <c r="K30" s="4">
+        <v>4.0565300442463599</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3">
+        <v>6</v>
+      </c>
+      <c r="N30" s="4">
+        <v>3.4512665853086801</v>
+      </c>
+      <c r="O30" s="4">
+        <v>3.60453870568523</v>
+      </c>
+      <c r="P30" s="4">
+        <v>4.0071647541010096</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>3.4181514655857801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>3</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>0</v>
+      </c>
+      <c r="B33" s="4">
+        <v>-9.5232153545961096E-2</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-9.4974799473283106E-2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>-9.7997128950280898E-2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>-9.7997128950280898E-2</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
         <v>8.2886840772579101E-2</v>
       </c>
-      <c r="C15" s="2">
+      <c r="I33" s="1">
         <v>0.17103346502717801</v>
       </c>
-      <c r="D15" s="2">
+      <c r="J33" s="1">
         <v>7.9411947826947701E-2</v>
       </c>
-      <c r="E15" s="2">
+      <c r="K33" s="1">
         <v>7.9411947826947701E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
         <v>1</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B34" s="4">
+        <v>-6.6483079752950897E-2</v>
+      </c>
+      <c r="C34" s="4">
+        <v>-6.5792428184403007E-2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>-6.7906222626308202E-2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>-6.5985273913957407E-2</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
         <v>7.3233118777663794E-2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="I34" s="1">
         <v>9.1202460112922004E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="J34" s="1">
         <v>0.100642505483282</v>
       </c>
-      <c r="E16" s="2">
+      <c r="K34" s="1">
         <v>0.34665806817838202</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
         <v>2</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B35" s="4">
+        <v>-0.17407538708690201</v>
+      </c>
+      <c r="C35" s="4">
+        <v>-0.17174428716530599</v>
+      </c>
+      <c r="D35" s="4">
+        <v>-0.170866398635656</v>
+      </c>
+      <c r="E35" s="4">
+        <v>-0.18839144240258099</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35" s="1">
         <v>0.32773886011508901</v>
       </c>
-      <c r="C17" s="2">
+      <c r="I35" s="1">
         <v>0.32998908306929797</v>
       </c>
-      <c r="D17" s="2">
+      <c r="J35" s="1">
         <v>0.34280317331933002</v>
       </c>
-      <c r="E17" s="2">
+      <c r="K35" s="1">
         <v>0.65640396646000199</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
         <v>3</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B36" s="4">
+        <v>-7.5705160969835206E-2</v>
+      </c>
+      <c r="C36" s="4">
+        <v>-7.2777916787026706E-2</v>
+      </c>
+      <c r="D36" s="4">
+        <v>-7.7557507911787005E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>-8.3790169567995398E-2</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36" s="1">
         <v>7.6544678130344698E-2</v>
       </c>
-      <c r="C18" s="2">
+      <c r="I36" s="1">
         <v>4.0877165516154598E-2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="J36" s="1">
         <v>8.68512905049139E-2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="K36" s="1">
         <v>0.48963051192453699</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
         <v>4</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B37" s="4">
+        <v>-5.4291249773693803E-2</v>
+      </c>
+      <c r="C37" s="4">
+        <v>-5.3640696870740301E-2</v>
+      </c>
+      <c r="D37" s="4">
+        <v>-5.6090292206924602E-2</v>
+      </c>
+      <c r="E37" s="4">
+        <v>-5.8092326129804597E-2</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1">
         <v>2.8493438220888598E-2</v>
       </c>
-      <c r="C19" s="2">
+      <c r="I37" s="1">
         <v>-5.4257468259765199E-2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="J37" s="1">
         <v>-3.0304428946621401E-2</v>
       </c>
-      <c r="E19" s="2">
+      <c r="K37" s="1">
         <v>2.6556981939126399E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
         <v>5</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B38" s="4">
+        <v>-0.10177066027727399</v>
+      </c>
+      <c r="C38" s="4">
+        <v>-0.104751225200349</v>
+      </c>
+      <c r="D38" s="4">
+        <v>-0.101749467006212</v>
+      </c>
+      <c r="E38" s="4">
+        <v>-0.100854273624618</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38" s="1">
         <v>0.104558356066043</v>
       </c>
-      <c r="C20" s="2">
+      <c r="I38" s="1">
         <v>2.5843066849393099E-2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="J38" s="1">
         <v>3.4069165607518499E-2</v>
       </c>
-      <c r="E20" s="2">
+      <c r="K38" s="1">
         <v>9.6999784588476606E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
         <v>6</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B39" s="4">
+        <v>-7.5056067937858295E-2</v>
+      </c>
+      <c r="C39" s="4">
+        <v>-7.0586312390407205E-2</v>
+      </c>
+      <c r="D39" s="4">
+        <v>-7.4377110369817506E-2</v>
+      </c>
+      <c r="E39" s="4">
+        <v>-7.2955320289390405E-2</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1">
         <v>4.9268760795150399E-2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="I39" s="1">
         <v>-6.7726767602601906E-2</v>
       </c>
-      <c r="D21" s="2">
+      <c r="J39" s="1">
         <v>3.6866427482193702E-2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="K39" s="1">
         <v>6.5250566843438801E-2</v>
       </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1988,7 +3005,259 @@
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:Y1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B15:E15">
+  <conditionalFormatting sqref="H33:K33">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:K34">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:K35">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:K36">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37:K37">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38:K38">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39:K39">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:K15 H17:K17 H19:K19 H21:K21">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:K16 H18:K18 H20:K20">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:E17 B15:E15 B19:E19 B21:E21">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:E16 B18:E18 B20:E20">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:K21">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:E21">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:Q15 N17:Q17 N19:Q19 N21:Q21">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:Q16 N18:Q18 N20:Q20">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:Q21">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:E24 B26:E26 B28:E28 B30:E30">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:E25 B27:E27 B29:E29">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:E30">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:K24 H26:K26 H28:K28 H30:K30">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:K25 H27:K27 H29:K29">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:K30">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2000,7 +3269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16">
+  <conditionalFormatting sqref="N24:Q24 N26:Q26 N28:Q28 N30:Q30">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2012,7 +3281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:E17">
+  <conditionalFormatting sqref="N25:Q25 N27:Q27 N29:Q29">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2024,7 +3293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:E18">
+  <conditionalFormatting sqref="N24:Q30">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2036,7 +3305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:E19">
+  <conditionalFormatting sqref="B33:E33 B35:E35 B37:E37 B39:E39">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2048,7 +3317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:E20">
+  <conditionalFormatting sqref="B34:E34 B36:E36 B38:E38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2060,7 +3329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:E21">
+  <conditionalFormatting sqref="B33:E39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>